<commit_message>
cleared the app for starters
</commit_message>
<xml_diff>
--- a/Data/data_model.xlsx
+++ b/Data/data_model.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Admin/Documents/GitHub/banner_magic/TEMPLATES/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Admin/Documents/GitHub/banner_magic/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60728349-A6A5-4844-B652-7BBB57E7D4CB}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E364367-67A9-B248-95BD-C6978EA0ADD7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,47 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>Bristan Basin Mixers</t>
-  </si>
-  <si>
-    <t>Bristan Bath Shower Mixers</t>
-  </si>
-  <si>
-    <t>Bristan Pillar Taps</t>
-  </si>
-  <si>
-    <t>Bristan Bath Fillers</t>
-  </si>
-  <si>
-    <t>Bristan Tap Spares</t>
-  </si>
-  <si>
-    <t>Bristan Digital Showers</t>
-  </si>
-  <si>
-    <t>Bristan Electric Showers</t>
-  </si>
-  <si>
-    <t>Bristan Shower Mixers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bristan Shower Cartridges </t>
-  </si>
-  <si>
-    <t>Bristan Shower Kits</t>
-  </si>
-  <si>
-    <t>Bristan Kitchen Taps</t>
-  </si>
-  <si>
-    <t>Bristan Accessories</t>
-  </si>
-  <si>
-    <t>Bristan Shower Heads &amp; Hoses</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -381,83 +341,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="22.5" customWidth="1"/>
   </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>